<commit_message>
Revert "Revert "AI ITEM""
This reverts commit c24b987dddbd33fa9a8fba97afd46f586acb0512.
</commit_message>
<xml_diff>
--- a/포폴작업현황.xlsx
+++ b/포폴작업현황.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\67728\Documents\Github\UnrealCPP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\67728\Documents\GitHub\UnrealCPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EBD24F-C46D-4CE1-BC19-B1528F31F6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEF5A36-9200-4F11-8A61-F5540B62847E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8DDB0EB3-E758-4E62-81CB-722328F53995}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8DDB0EB3-E758-4E62-81CB-722328F53995}"/>
   </bookViews>
   <sheets>
     <sheet name="작업일지" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="204">
   <si>
     <t>10월27일</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1333,6 +1333,50 @@
   <si>
     <t>AI
 AI_Behavior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기본 캐릭터 구조
+PushingComponent
+(SphereComponent 상속)
+HP UI
+Citem
+CEquipActor
+CEquipActor_Dual
+StateComponent+BE5
+CWeaponAsset
+CDoAction
+Cequipment
+StatusCompoent
+CSkill
+CSkill_Passive
+CSkill_Active
+CSlashProjectile
+CSkill_Active_Slash
+CSkill_Active_Throw
+CBoomerang_Thorw+CC5
+CDropItem
+InventoryComponent
+InventoryWidget
+HitWidget
+Ridding+CI5
+Jump
+Bow_Skill
+Bow
+SkillComponent
+SkillTree_Widget
+Widget 구조 변경
+Widget TitleBar
+QuickSlotComponent
+QuickSlotWidget
+DashSkill
+SkillCombo
+AI_Behavior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AI
+원거리 무기, AI 추가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1476,9 +1520,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1486,15 +1527,18 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1814,16 +1858,16 @@
   <dimension ref="A2:DC6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BZ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CF2" sqref="CF2:CF6"/>
+      <pane xSplit="1" topLeftCell="CE1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CH2" sqref="CH2:CH6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="98" width="30.75" customWidth="1"/>
+    <col min="2" max="98" width="30.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:107" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -2117,7 +2161,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="3" spans="1:107" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:107" ht="87" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
@@ -2364,8 +2408,14 @@
       <c r="CH3" s="2" t="s">
         <v>150</v>
       </c>
+      <c r="CI3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CJ3" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="4" spans="1:107" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:107" ht="90" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
@@ -2612,8 +2662,14 @@
       <c r="CH4" s="2" t="s">
         <v>201</v>
       </c>
+      <c r="CI4" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="CJ4" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
-    <row r="5" spans="1:107" ht="408.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:107" ht="408.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -2747,142 +2803,146 @@
       <c r="AS5" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="AT5" s="11" t="s">
+      <c r="AT5" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AU5" s="11" t="s">
+      <c r="AU5" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="AV5" s="11" t="s">
+      <c r="AV5" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="AW5" s="11" t="s">
+      <c r="AW5" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="AX5" s="11" t="s">
+      <c r="AX5" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="AY5" s="11" t="s">
+      <c r="AY5" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="AZ5" s="13"/>
-      <c r="BA5" s="13"/>
-      <c r="BB5" s="11" t="s">
+      <c r="AZ5" s="14"/>
+      <c r="BA5" s="14"/>
+      <c r="BB5" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="BC5" s="11" t="s">
+      <c r="BC5" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="BD5" s="11" t="s">
+      <c r="BD5" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="BE5" s="11" t="s">
+      <c r="BE5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="BF5" s="11" t="s">
+      <c r="BF5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="BG5" s="11" t="s">
+      <c r="BG5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="BH5" s="11" t="s">
+      <c r="BH5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="BI5" s="15"/>
-      <c r="BJ5" s="11" t="s">
+      <c r="BI5" s="12"/>
+      <c r="BJ5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="BK5" s="11" t="s">
+      <c r="BK5" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="BL5" s="11" t="s">
+      <c r="BL5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BM5" s="11" t="s">
+      <c r="BM5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BN5" s="11" t="s">
+      <c r="BN5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BO5" s="11" t="s">
+      <c r="BO5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BP5" s="11" t="s">
+      <c r="BP5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BQ5" s="11" t="s">
+      <c r="BQ5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BR5" s="11" t="s">
+      <c r="BR5" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="BS5" s="11" t="s">
+      <c r="BS5" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BT5" s="11" t="s">
+      <c r="BT5" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BU5" s="11" t="s">
+      <c r="BU5" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BV5" s="11" t="s">
+      <c r="BV5" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BW5" s="11" t="s">
+      <c r="BW5" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BX5" s="11" t="s">
+      <c r="BX5" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="BY5" s="11" t="s">
+      <c r="BY5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="BZ5" s="11" t="s">
+      <c r="BZ5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="CA5" s="11" t="s">
+      <c r="CA5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="CB5" s="11" t="s">
+      <c r="CB5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="CC5" s="11" t="s">
+      <c r="CC5" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="CD5" s="10"/>
-      <c r="CE5" s="10"/>
-      <c r="CF5" s="11" t="s">
+      <c r="CD5" s="16"/>
+      <c r="CE5" s="16"/>
+      <c r="CF5" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="CG5" s="11" t="s">
+      <c r="CG5" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="CH5" s="11" t="s">
+      <c r="CH5" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="CI5" s="10"/>
-      <c r="CJ5" s="10"/>
-      <c r="CK5" s="10"/>
-      <c r="CL5" s="10"/>
-      <c r="CM5" s="10"/>
-      <c r="CN5" s="10"/>
-      <c r="CO5" s="10"/>
-      <c r="CP5" s="10"/>
-      <c r="CQ5" s="10"/>
-      <c r="CR5" s="10"/>
-      <c r="CS5" s="10"/>
-      <c r="CT5" s="10"/>
-      <c r="CU5" s="10"/>
-      <c r="CV5" s="10"/>
-      <c r="CW5" s="10"/>
-      <c r="CX5" s="10"/>
-      <c r="CY5" s="10"/>
-      <c r="CZ5" s="10"/>
-      <c r="DA5" s="10"/>
-      <c r="DB5" s="10"/>
-      <c r="DC5" s="10"/>
+      <c r="CI5" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="CJ5" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="CK5" s="16"/>
+      <c r="CL5" s="16"/>
+      <c r="CM5" s="16"/>
+      <c r="CN5" s="16"/>
+      <c r="CO5" s="16"/>
+      <c r="CP5" s="16"/>
+      <c r="CQ5" s="16"/>
+      <c r="CR5" s="16"/>
+      <c r="CS5" s="16"/>
+      <c r="CT5" s="16"/>
+      <c r="CU5" s="16"/>
+      <c r="CV5" s="16"/>
+      <c r="CW5" s="16"/>
+      <c r="CX5" s="16"/>
+      <c r="CY5" s="16"/>
+      <c r="CZ5" s="16"/>
+      <c r="DA5" s="16"/>
+      <c r="DB5" s="16"/>
+      <c r="DC5" s="16"/>
     </row>
-    <row r="6" spans="1:107" ht="309" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:107" ht="309" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -2927,133 +2987,133 @@
       <c r="AQ6" s="8"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8"/>
-      <c r="AT6" s="12"/>
-      <c r="AU6" s="12"/>
-      <c r="AV6" s="12"/>
-      <c r="AW6" s="12"/>
-      <c r="AX6" s="12"/>
-      <c r="AY6" s="12"/>
-      <c r="AZ6" s="14"/>
-      <c r="BA6" s="14"/>
-      <c r="BB6" s="12"/>
-      <c r="BC6" s="12"/>
-      <c r="BD6" s="12"/>
-      <c r="BE6" s="12"/>
-      <c r="BF6" s="12"/>
-      <c r="BG6" s="12"/>
-      <c r="BH6" s="12"/>
-      <c r="BI6" s="16"/>
-      <c r="BJ6" s="12"/>
-      <c r="BK6" s="12"/>
-      <c r="BL6" s="12"/>
-      <c r="BM6" s="12"/>
-      <c r="BN6" s="12"/>
-      <c r="BO6" s="12"/>
-      <c r="BP6" s="12"/>
-      <c r="BQ6" s="12"/>
-      <c r="BR6" s="12"/>
-      <c r="BS6" s="12"/>
-      <c r="BT6" s="12"/>
-      <c r="BU6" s="12"/>
-      <c r="BV6" s="12"/>
-      <c r="BW6" s="12"/>
-      <c r="BX6" s="12"/>
-      <c r="BY6" s="12"/>
-      <c r="BZ6" s="12"/>
-      <c r="CA6" s="12"/>
-      <c r="CB6" s="12"/>
-      <c r="CC6" s="12"/>
-      <c r="CD6" s="10"/>
-      <c r="CE6" s="10"/>
-      <c r="CF6" s="12"/>
-      <c r="CG6" s="12"/>
-      <c r="CH6" s="12"/>
-      <c r="CI6" s="10"/>
-      <c r="CJ6" s="10"/>
-      <c r="CK6" s="10"/>
-      <c r="CL6" s="10"/>
-      <c r="CM6" s="10"/>
-      <c r="CN6" s="10"/>
-      <c r="CO6" s="10"/>
-      <c r="CP6" s="10"/>
-      <c r="CQ6" s="10"/>
-      <c r="CR6" s="10"/>
-      <c r="CS6" s="10"/>
-      <c r="CT6" s="10"/>
-      <c r="CU6" s="10"/>
-      <c r="CV6" s="10"/>
-      <c r="CW6" s="10"/>
-      <c r="CX6" s="10"/>
-      <c r="CY6" s="10"/>
-      <c r="CZ6" s="10"/>
-      <c r="DA6" s="10"/>
-      <c r="DB6" s="10"/>
-      <c r="DC6" s="10"/>
+      <c r="AT6" s="11"/>
+      <c r="AU6" s="11"/>
+      <c r="AV6" s="11"/>
+      <c r="AW6" s="11"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="11"/>
+      <c r="AZ6" s="15"/>
+      <c r="BA6" s="15"/>
+      <c r="BB6" s="11"/>
+      <c r="BC6" s="11"/>
+      <c r="BD6" s="11"/>
+      <c r="BE6" s="11"/>
+      <c r="BF6" s="11"/>
+      <c r="BG6" s="11"/>
+      <c r="BH6" s="11"/>
+      <c r="BI6" s="13"/>
+      <c r="BJ6" s="11"/>
+      <c r="BK6" s="11"/>
+      <c r="BL6" s="11"/>
+      <c r="BM6" s="11"/>
+      <c r="BN6" s="11"/>
+      <c r="BO6" s="11"/>
+      <c r="BP6" s="11"/>
+      <c r="BQ6" s="11"/>
+      <c r="BR6" s="11"/>
+      <c r="BS6" s="11"/>
+      <c r="BT6" s="11"/>
+      <c r="BU6" s="11"/>
+      <c r="BV6" s="11"/>
+      <c r="BW6" s="11"/>
+      <c r="BX6" s="11"/>
+      <c r="BY6" s="11"/>
+      <c r="BZ6" s="11"/>
+      <c r="CA6" s="11"/>
+      <c r="CB6" s="11"/>
+      <c r="CC6" s="11"/>
+      <c r="CD6" s="16"/>
+      <c r="CE6" s="16"/>
+      <c r="CF6" s="11"/>
+      <c r="CG6" s="11"/>
+      <c r="CH6" s="11"/>
+      <c r="CI6" s="11"/>
+      <c r="CJ6" s="11"/>
+      <c r="CK6" s="16"/>
+      <c r="CL6" s="16"/>
+      <c r="CM6" s="16"/>
+      <c r="CN6" s="16"/>
+      <c r="CO6" s="16"/>
+      <c r="CP6" s="16"/>
+      <c r="CQ6" s="16"/>
+      <c r="CR6" s="16"/>
+      <c r="CS6" s="16"/>
+      <c r="CT6" s="16"/>
+      <c r="CU6" s="16"/>
+      <c r="CV6" s="16"/>
+      <c r="CW6" s="16"/>
+      <c r="CX6" s="16"/>
+      <c r="CY6" s="16"/>
+      <c r="CZ6" s="16"/>
+      <c r="DA6" s="16"/>
+      <c r="DB6" s="16"/>
+      <c r="DC6" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="CY5:CY6"/>
+    <mergeCell ref="CZ5:CZ6"/>
+    <mergeCell ref="DA5:DA6"/>
+    <mergeCell ref="DB5:DB6"/>
+    <mergeCell ref="DC5:DC6"/>
+    <mergeCell ref="CT5:CT6"/>
+    <mergeCell ref="CU5:CU6"/>
+    <mergeCell ref="CV5:CV6"/>
+    <mergeCell ref="CW5:CW6"/>
+    <mergeCell ref="CX5:CX6"/>
+    <mergeCell ref="CO5:CO6"/>
+    <mergeCell ref="CP5:CP6"/>
+    <mergeCell ref="CQ5:CQ6"/>
+    <mergeCell ref="CR5:CR6"/>
+    <mergeCell ref="CS5:CS6"/>
+    <mergeCell ref="CJ5:CJ6"/>
+    <mergeCell ref="CK5:CK6"/>
+    <mergeCell ref="CL5:CL6"/>
+    <mergeCell ref="CM5:CM6"/>
+    <mergeCell ref="CN5:CN6"/>
+    <mergeCell ref="CE5:CE6"/>
+    <mergeCell ref="CF5:CF6"/>
+    <mergeCell ref="CG5:CG6"/>
+    <mergeCell ref="CH5:CH6"/>
+    <mergeCell ref="CI5:CI6"/>
+    <mergeCell ref="BZ5:BZ6"/>
+    <mergeCell ref="CA5:CA6"/>
+    <mergeCell ref="CB5:CB6"/>
+    <mergeCell ref="CC5:CC6"/>
+    <mergeCell ref="CD5:CD6"/>
+    <mergeCell ref="BU5:BU6"/>
+    <mergeCell ref="BV5:BV6"/>
+    <mergeCell ref="BW5:BW6"/>
+    <mergeCell ref="BX5:BX6"/>
+    <mergeCell ref="BY5:BY6"/>
+    <mergeCell ref="BP5:BP6"/>
+    <mergeCell ref="BQ5:BQ6"/>
+    <mergeCell ref="BR5:BR6"/>
+    <mergeCell ref="BS5:BS6"/>
+    <mergeCell ref="BT5:BT6"/>
+    <mergeCell ref="AY5:AY6"/>
+    <mergeCell ref="AW5:AW6"/>
+    <mergeCell ref="AV5:AV6"/>
+    <mergeCell ref="AU5:AU6"/>
+    <mergeCell ref="AT5:AT6"/>
+    <mergeCell ref="AX5:AX6"/>
+    <mergeCell ref="AZ5:AZ6"/>
+    <mergeCell ref="BA5:BA6"/>
+    <mergeCell ref="BB5:BB6"/>
+    <mergeCell ref="BC5:BC6"/>
+    <mergeCell ref="BD5:BD6"/>
+    <mergeCell ref="BE5:BE6"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BH5:BH6"/>
+    <mergeCell ref="BI5:BI6"/>
     <mergeCell ref="BO5:BO6"/>
     <mergeCell ref="BJ5:BJ6"/>
     <mergeCell ref="BK5:BK6"/>
     <mergeCell ref="BL5:BL6"/>
     <mergeCell ref="BM5:BM6"/>
     <mergeCell ref="BN5:BN6"/>
-    <mergeCell ref="BE5:BE6"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BH5:BH6"/>
-    <mergeCell ref="BI5:BI6"/>
-    <mergeCell ref="AZ5:AZ6"/>
-    <mergeCell ref="BA5:BA6"/>
-    <mergeCell ref="BB5:BB6"/>
-    <mergeCell ref="BC5:BC6"/>
-    <mergeCell ref="BD5:BD6"/>
-    <mergeCell ref="AY5:AY6"/>
-    <mergeCell ref="AW5:AW6"/>
-    <mergeCell ref="AV5:AV6"/>
-    <mergeCell ref="AU5:AU6"/>
-    <mergeCell ref="AT5:AT6"/>
-    <mergeCell ref="AX5:AX6"/>
-    <mergeCell ref="BP5:BP6"/>
-    <mergeCell ref="BQ5:BQ6"/>
-    <mergeCell ref="BR5:BR6"/>
-    <mergeCell ref="BS5:BS6"/>
-    <mergeCell ref="BT5:BT6"/>
-    <mergeCell ref="BU5:BU6"/>
-    <mergeCell ref="BV5:BV6"/>
-    <mergeCell ref="BW5:BW6"/>
-    <mergeCell ref="BX5:BX6"/>
-    <mergeCell ref="BY5:BY6"/>
-    <mergeCell ref="BZ5:BZ6"/>
-    <mergeCell ref="CA5:CA6"/>
-    <mergeCell ref="CB5:CB6"/>
-    <mergeCell ref="CC5:CC6"/>
-    <mergeCell ref="CD5:CD6"/>
-    <mergeCell ref="CE5:CE6"/>
-    <mergeCell ref="CF5:CF6"/>
-    <mergeCell ref="CG5:CG6"/>
-    <mergeCell ref="CH5:CH6"/>
-    <mergeCell ref="CI5:CI6"/>
-    <mergeCell ref="CJ5:CJ6"/>
-    <mergeCell ref="CK5:CK6"/>
-    <mergeCell ref="CL5:CL6"/>
-    <mergeCell ref="CM5:CM6"/>
-    <mergeCell ref="CN5:CN6"/>
-    <mergeCell ref="CO5:CO6"/>
-    <mergeCell ref="CP5:CP6"/>
-    <mergeCell ref="CQ5:CQ6"/>
-    <mergeCell ref="CR5:CR6"/>
-    <mergeCell ref="CS5:CS6"/>
-    <mergeCell ref="CT5:CT6"/>
-    <mergeCell ref="CU5:CU6"/>
-    <mergeCell ref="CV5:CV6"/>
-    <mergeCell ref="CW5:CW6"/>
-    <mergeCell ref="CX5:CX6"/>
-    <mergeCell ref="CY5:CY6"/>
-    <mergeCell ref="CZ5:CZ6"/>
-    <mergeCell ref="DA5:DA6"/>
-    <mergeCell ref="DB5:DB6"/>
-    <mergeCell ref="DC5:DC6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3069,24 +3129,24 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="7" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="8:12" x14ac:dyDescent="0.4">
       <c r="K9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="8:12" x14ac:dyDescent="0.4">
       <c r="K10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H11" t="s">
         <v>127</v>
       </c>
@@ -3094,37 +3154,37 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H12" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H13" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="8:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="8:12" x14ac:dyDescent="0.4">
       <c r="H16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.4">
       <c r="H17" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.4">
       <c r="H18" t="s">
         <v>134</v>
       </c>

</xml_diff>